<commit_message>
Aggiornata specifica, aggiunta Verifica dei requisiti funzionali
</commit_message>
<xml_diff>
--- a/RR/Esterni/Analisi dei Requisiti/Specifica/specifica.xlsx
+++ b/RR/Esterni/Analisi dei Requisiti/Specifica/specifica.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="28695" windowHeight="12810"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="282">
   <si>
     <t>Table 1</t>
   </si>
@@ -448,10 +450,6 @@
     <t>RF13</t>
   </si>
   <si>
-    <t xml:space="preserve">L’utente, all’interno del server, deve avere 3 cartelle diverse che contengono una solo le presentazioni, una solo le infografiche ed una solo le immagini 
-</t>
-  </si>
-  <si>
     <t>UC1.7
 UC1.12</t>
   </si>
@@ -501,9 +499,6 @@
     <t>L'utente deve essere in grado di spostare le proprie infografiche all’interno della cartella dedicata sul suo spazio nel server</t>
   </si>
   <si>
-    <t>MANCANTE</t>
-  </si>
-  <si>
     <t>RF34</t>
   </si>
   <si>
@@ -576,25 +571,16 @@
     <t>RF55</t>
   </si>
   <si>
-    <t>L'utente deve essere in grado di visualizzare una presentazione salvata sul server</t>
-  </si>
-  <si>
     <t>UC1.5</t>
   </si>
   <si>
     <t>RF58</t>
   </si>
   <si>
-    <t>L'utente deve essere in grado di visualizzare una presentazione salvata in locale</t>
-  </si>
-  <si>
     <t>UC1.14</t>
   </si>
   <si>
     <t>UC1.18</t>
-  </si>
-  <si>
-    <t>INDICI DA SCALARE</t>
   </si>
   <si>
     <t>-&gt;RF61.1</t>
@@ -628,9 +614,6 @@
     <t>--&gt;RF61.1.3</t>
   </si>
   <si>
-    <t>L'utente deve essere in grado di spostare la presentazione al frame più significativo successivo o precedente</t>
-  </si>
-  <si>
     <t>UC 1.18.1.3</t>
   </si>
   <si>
@@ -739,52 +722,6 @@
     <t>UC 1.18.2.5</t>
   </si>
   <si>
-    <t>--&gt;RF61.3.4</t>
-  </si>
-  <si>
-    <t>L'utente deve essere in grado di gestire la visualizzazione degli elementi multimediali</t>
-  </si>
-  <si>
-    <t>UC 1.18.2.6</t>
-  </si>
-  <si>
-    <t>---&gt;RF61.3.4.1</t>
-  </si>
-  <si>
-    <t>UC 1.18.2.6.1</t>
-  </si>
-  <si>
-    <t>---&gt;RF61.3.4.2</t>
-  </si>
-  <si>
-    <t>UC 1.18.2.6.2
-UC 1.18.2.6.3</t>
-  </si>
-  <si>
-    <t>---&gt;RF61.3.4.3</t>
-  </si>
-  <si>
-    <t>UC 1.18.2.6.4</t>
-  </si>
-  <si>
-    <t>---&gt;RF61.3.4.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L'utente deve essere in grado di  saltare la visualizzazione del video </t>
-  </si>
-  <si>
-    <t>UC 1.18.2.6.5</t>
-  </si>
-  <si>
-    <t>---&gt;RF61.3.4.5</t>
-  </si>
-  <si>
-    <t>L'utente deve essere in grado di aumentare le dimensioni del video</t>
-  </si>
-  <si>
-    <t>UC 1.18.2.6.6</t>
-  </si>
-  <si>
     <t>-&gt;RF61.4</t>
   </si>
   <si>
@@ -812,14 +749,7 @@
     <t>L'utente deve essere in grado una volta autenticato si effettuare il logout dal server e passare alla modalità offline</t>
   </si>
   <si>
-    <t>UC1.9
-INTEGRARE</t>
-  </si>
-  <si>
     <t>RF67</t>
-  </si>
-  <si>
-    <t>L'utente amministratore deve essere in grado di gestire alcune funzionalità a livello back-end</t>
   </si>
   <si>
     <t>UC 1.9</t>
@@ -948,15 +878,34 @@
   <si>
     <t>UC 1.9.7.3</t>
   </si>
+  <si>
+    <t>L'utente amministratore deve essere in grado di passare nella modalità per gestire alcune funzionalità a livello back-end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’utente, all’interno del proprio spazio del server, deve avere 3 cartelle diverse che contengono una solo le presentazioni, una solo le infografiche ed una solo le immagini 
+</t>
+  </si>
+  <si>
+    <t>UC1.7.6</t>
+  </si>
+  <si>
+    <t>UC1.7.7</t>
+  </si>
+  <si>
+    <t>L'utente deve essere in grado di eseguire una presentazione salvata sul server</t>
+  </si>
+  <si>
+    <t>L'utente deve essere in grado di eseguire una presentazione salvata in locale</t>
+  </si>
+  <si>
+    <t>L'utente deve essere in grado di spostare la presentazione al frame con bookmark successivo o precedente</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -973,12 +922,7 @@
       <name val="Verdana"/>
     </font>
     <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
@@ -1100,99 +1044,152 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="7" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ffffe061"/>
-      <rgbColor rgb="fffefefe"/>
-      <rgbColor rgb="ff9ce159"/>
-      <rgbColor rgb="ff6dc037"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FFFFE061"/>
+      <rgbColor rgb="FFFEFEFE"/>
+      <rgbColor rgb="FF9CE159"/>
+      <rgbColor rgb="FF6DC037"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -1384,7 +1381,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -1393,7 +1390,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -1402,7 +1399,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -1411,7 +1408,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1420,7 +1417,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1429,7 +1426,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1541,8 +1538,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -1550,14 +1547,14 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1576,7 +1573,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1584,7 +1581,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -1612,7 +1609,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1638,7 +1635,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1664,7 +1661,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1690,7 +1687,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1716,7 +1713,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1742,7 +1739,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1768,7 +1765,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1794,7 +1791,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1820,7 +1817,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1833,9 +1830,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1851,7 +1854,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1870,7 +1873,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1896,7 +1899,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1922,7 +1925,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1948,7 +1951,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1974,7 +1977,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2000,7 +2003,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2026,7 +2029,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2052,7 +2055,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2078,7 +2081,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2104,7 +2107,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2117,9 +2120,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -2132,7 +2141,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2151,7 +2160,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2181,7 +2190,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2207,7 +2216,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2233,7 +2242,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2259,7 +2268,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2285,7 +2294,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2311,7 +2320,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2337,7 +2346,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2363,7 +2372,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2389,7 +2398,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2402,1926 +2411,1878 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H109"/>
+  <dimension ref="A1:IV109"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.09765625" style="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.09765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.3984375" style="1" customWidth="1"/>
+    <col min="5" max="8" width="9.09765625" style="1" customWidth="1"/>
     <col min="9" max="256" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" ht="20.55" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" t="s" s="7">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s" s="7">
+      <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s" s="7">
+      <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s" s="7">
+      <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-    </row>
-    <row r="4" ht="86.9" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" t="s" s="7">
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" ht="86.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s" s="7">
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s" s="7">
+      <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s" s="7">
+      <c r="E4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-    </row>
-    <row r="5" ht="44.35" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" t="s" s="7">
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s" s="7">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s" s="7">
+      <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s" s="7">
+      <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" ht="44.35" customHeight="1">
-      <c r="A6" s="6"/>
-      <c r="B6" t="s" s="7">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s" s="7">
+      <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s" s="7">
+      <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s" s="7">
+      <c r="E6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-    </row>
-    <row r="7" ht="72.35" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" t="s" s="7">
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="72.400000000000006" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s" s="7">
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s" s="7">
+      <c r="D7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s" s="7">
+      <c r="E7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-    </row>
-    <row r="8" ht="44.35" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" t="s" s="7">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s" s="7">
+      <c r="C8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s" s="7">
+      <c r="D8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E8" t="s" s="7">
+      <c r="E8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" ht="44.35" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" t="s" s="7">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C9" t="s" s="7">
+      <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D9" t="s" s="7">
+      <c r="D9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E9" t="s" s="7">
+      <c r="E9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" ht="32.35" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" t="s" s="7">
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C10" t="s" s="7">
+      <c r="C10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D10" t="s" s="7">
+      <c r="D10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E10" t="s" s="7">
+      <c r="E10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" ht="32.35" customHeight="1">
-      <c r="A11" s="6"/>
-      <c r="B11" t="s" s="7">
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C11" t="s" s="7">
+      <c r="C11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D11" t="s" s="7">
+      <c r="D11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E11" t="s" s="7">
+      <c r="E11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" ht="44.35" customHeight="1">
-      <c r="A12" s="6"/>
-      <c r="B12" t="s" s="7">
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C12" t="s" s="7">
+      <c r="C12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D12" t="s" s="7">
+      <c r="D12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E12" t="s" s="7">
+      <c r="E12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" ht="56.35" customHeight="1">
-      <c r="A13" s="6"/>
-      <c r="B13" t="s" s="7">
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" ht="56.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C13" t="s" s="7">
+      <c r="C13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D13" t="s" s="7">
+      <c r="D13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E13" t="s" s="7">
+      <c r="E13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" ht="32.35" customHeight="1">
-      <c r="A14" s="6"/>
-      <c r="B14" t="s" s="7">
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C14" t="s" s="7">
+      <c r="C14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D14" t="s" s="7">
+      <c r="D14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E14" t="s" s="7">
+      <c r="E14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" ht="44.35" customHeight="1">
-      <c r="A15" s="6"/>
-      <c r="B15" t="s" s="7">
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C15" t="s" s="7">
+      <c r="C15" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D15" t="s" s="7">
+      <c r="D15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E15" t="s" s="7">
+      <c r="E15" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-    </row>
-    <row r="16" ht="56.35" customHeight="1">
-      <c r="A16" s="6"/>
-      <c r="B16" t="s" s="7">
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" ht="56.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C16" t="s" s="7">
+      <c r="C16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D16" t="s" s="7">
+      <c r="D16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E16" t="s" s="7">
+      <c r="E16" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" ht="56.35" customHeight="1">
-      <c r="A17" s="6"/>
-      <c r="B17" t="s" s="7">
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" ht="56.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C17" t="s" s="7">
+      <c r="C17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D17" t="s" s="7">
+      <c r="D17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E17" t="s" s="7">
+      <c r="E17" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-    </row>
-    <row r="18" ht="44.35" customHeight="1">
-      <c r="A18" s="6"/>
-      <c r="B18" t="s" s="7">
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C18" t="s" s="7">
+      <c r="C18" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D18" t="s" s="7">
+      <c r="D18" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E18" t="s" s="7">
+      <c r="E18" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-    </row>
-    <row r="19" ht="32.35" customHeight="1">
-      <c r="A19" s="6"/>
-      <c r="B19" t="s" s="7">
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C19" t="s" s="7">
+      <c r="C19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D19" t="s" s="7">
+      <c r="D19" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E19" t="s" s="7">
+      <c r="E19" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-    </row>
-    <row r="20" ht="32.35" customHeight="1">
-      <c r="A20" s="6"/>
-      <c r="B20" t="s" s="7">
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C20" t="s" s="7">
+      <c r="C20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D20" t="s" s="7">
+      <c r="D20" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E20" t="s" s="7">
+      <c r="E20" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-    </row>
-    <row r="21" ht="44.35" customHeight="1">
-      <c r="A21" s="6"/>
-      <c r="B21" t="s" s="7">
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C21" t="s" s="7">
+      <c r="C21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D21" t="s" s="7">
+      <c r="D21" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E21" t="s" s="7">
+      <c r="E21" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-    </row>
-    <row r="22" ht="44.35" customHeight="1">
-      <c r="A22" s="6"/>
-      <c r="B22" t="s" s="7">
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C22" t="s" s="7">
+      <c r="C22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D22" t="s" s="7">
+      <c r="D22" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E22" t="s" s="7">
+      <c r="E22" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-    </row>
-    <row r="23" ht="44.35" customHeight="1">
-      <c r="A23" s="6"/>
-      <c r="B23" t="s" s="7">
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C23" t="s" s="7">
+      <c r="C23" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D23" t="s" s="7">
+      <c r="D23" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E23" t="s" s="7">
+      <c r="E23" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-    </row>
-    <row r="24" ht="44.35" customHeight="1">
-      <c r="A24" s="6"/>
-      <c r="B24" t="s" s="7">
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C24" t="s" s="7">
+      <c r="C24" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D24" t="s" s="7">
+      <c r="D24" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E24" t="s" s="7">
+      <c r="E24" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-    </row>
-    <row r="25" ht="44.35" customHeight="1">
-      <c r="A25" s="6"/>
-      <c r="B25" t="s" s="7">
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C25" t="s" s="7">
+      <c r="C25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D25" t="s" s="7">
+      <c r="D25" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E25" t="s" s="7">
+      <c r="E25" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-    </row>
-    <row r="26" ht="68.35" customHeight="1">
-      <c r="A26" s="6"/>
-      <c r="B26" t="s" s="7">
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" ht="68.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="B26" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C26" t="s" s="7">
+      <c r="C26" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D26" t="s" s="7">
+      <c r="D26" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E26" t="s" s="7">
+      <c r="E26" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-    </row>
-    <row r="27" ht="68.35" customHeight="1">
-      <c r="A27" s="6"/>
-      <c r="B27" t="s" s="7">
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" ht="68.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C27" t="s" s="7">
+      <c r="C27" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D27" t="s" s="7">
+      <c r="D27" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E27" t="s" s="7">
+      <c r="E27" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-    </row>
-    <row r="28" ht="44.35" customHeight="1">
-      <c r="A28" s="6"/>
-      <c r="B28" t="s" s="7">
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+      <c r="B28" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C28" t="s" s="7">
+      <c r="C28" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D28" t="s" s="7">
+      <c r="D28" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E28" t="s" s="7">
+      <c r="E28" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-    </row>
-    <row r="29" ht="56.35" customHeight="1">
-      <c r="A29" s="6"/>
-      <c r="B29" t="s" s="7">
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" ht="56.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+      <c r="B29" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C29" t="s" s="7">
+      <c r="C29" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D29" t="s" s="7">
+      <c r="D29" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E29" t="s" s="7">
+      <c r="E29" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-    </row>
-    <row r="30" ht="44.35" customHeight="1">
-      <c r="A30" s="6"/>
-      <c r="B30" t="s" s="7">
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3"/>
+      <c r="B30" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C30" t="s" s="7">
+      <c r="C30" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D30" t="s" s="7">
+      <c r="D30" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E30" t="s" s="7">
+      <c r="E30" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-    </row>
-    <row r="31" ht="44.35" customHeight="1">
-      <c r="A31" s="6"/>
-      <c r="B31" t="s" s="7">
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3"/>
+      <c r="B31" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C31" t="s" s="7">
+      <c r="C31" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D31" t="s" s="7">
+      <c r="D31" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E31" t="s" s="7">
+      <c r="E31" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-    </row>
-    <row r="32" ht="44.35" customHeight="1">
-      <c r="A32" s="6"/>
-      <c r="B32" t="s" s="7">
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3"/>
+      <c r="B32" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C32" t="s" s="7">
+      <c r="C32" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D32" t="s" s="7">
+      <c r="D32" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E32" t="s" s="7">
+      <c r="E32" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-    </row>
-    <row r="33" ht="44.35" customHeight="1">
-      <c r="A33" s="6"/>
-      <c r="B33" t="s" s="7">
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3"/>
+      <c r="B33" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C33" t="s" s="7">
+      <c r="C33" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D33" t="s" s="7">
+      <c r="D33" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E33" t="s" s="7">
+      <c r="E33" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-    </row>
-    <row r="34" ht="44.35" customHeight="1">
-      <c r="A34" s="6"/>
-      <c r="B34" t="s" s="7">
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3"/>
+      <c r="B34" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C34" t="s" s="7">
+      <c r="C34" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D34" t="s" s="7">
+      <c r="D34" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E34" t="s" s="7">
+      <c r="E34" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-    </row>
-    <row r="35" ht="44.35" customHeight="1">
-      <c r="A35" s="6"/>
-      <c r="B35" t="s" s="7">
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3"/>
+      <c r="B35" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C35" t="s" s="7">
+      <c r="C35" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D35" t="s" s="7">
+      <c r="D35" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E35" t="s" s="7">
+      <c r="E35" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-    </row>
-    <row r="36" ht="44.35" customHeight="1">
-      <c r="A36" s="6"/>
-      <c r="B36" t="s" s="7">
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="3"/>
+      <c r="B36" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C36" t="s" s="7">
+      <c r="C36" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D36" t="s" s="7">
+      <c r="D36" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E36" t="s" s="7">
+      <c r="E36" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-    </row>
-    <row r="37" ht="44.35" customHeight="1">
-      <c r="A37" s="6"/>
-      <c r="B37" t="s" s="7">
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3"/>
+      <c r="B37" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C37" t="s" s="7">
+      <c r="C37" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D37" t="s" s="7">
+      <c r="D37" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E37" t="s" s="7">
+      <c r="E37" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-    </row>
-    <row r="38" ht="56.35" customHeight="1">
-      <c r="A38" s="6"/>
-      <c r="B38" t="s" s="7">
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+    </row>
+    <row r="38" spans="1:8" ht="56.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3"/>
+      <c r="B38" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C38" t="s" s="7">
+      <c r="C38" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D38" t="s" s="7">
+      <c r="D38" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E38" t="s" s="7">
+      <c r="E38" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-    </row>
-    <row r="39" ht="44.35" customHeight="1">
-      <c r="A39" s="6"/>
-      <c r="B39" t="s" s="7">
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="3"/>
+      <c r="B39" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C39" t="s" s="7">
+      <c r="C39" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D39" t="s" s="7">
+      <c r="D39" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E39" t="s" s="7">
+      <c r="E39" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-    </row>
-    <row r="40" ht="20.35" customHeight="1">
-      <c r="A40" s="6"/>
-      <c r="B40" t="s" s="7">
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3"/>
+      <c r="B40" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-    </row>
-    <row r="41" ht="44.35" customHeight="1">
-      <c r="A41" s="6"/>
-      <c r="B41" t="s" s="7">
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="3"/>
+      <c r="B41" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C41" t="s" s="7">
+      <c r="C41" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D41" t="s" s="7">
+      <c r="D41" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E41" t="s" s="7">
+      <c r="E41" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-    </row>
-    <row r="42" ht="44.35" customHeight="1">
-      <c r="A42" s="6"/>
-      <c r="B42" t="s" s="7">
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="3"/>
+      <c r="B42" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C42" t="s" s="7">
+      <c r="C42" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D42" t="s" s="7">
+      <c r="D42" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E42" t="s" s="7">
+      <c r="E42" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-    </row>
-    <row r="43" ht="44.35" customHeight="1">
-      <c r="A43" s="6"/>
-      <c r="B43" t="s" s="7">
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="3"/>
+      <c r="B43" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C43" t="s" s="7">
+      <c r="C43" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D43" t="s" s="7">
+      <c r="D43" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E43" t="s" s="7">
+      <c r="E43" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-    </row>
-    <row r="44" ht="44.35" customHeight="1">
-      <c r="A44" s="6"/>
-      <c r="B44" t="s" s="7">
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="3"/>
+      <c r="B44" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C44" t="s" s="7">
+      <c r="C44" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D44" t="s" s="7">
+      <c r="D44" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E44" t="s" s="7">
+      <c r="E44" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-    </row>
-    <row r="45" ht="44.35" customHeight="1">
-      <c r="A45" s="6"/>
-      <c r="B45" t="s" s="7">
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+    </row>
+    <row r="45" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="3"/>
+      <c r="B45" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C45" t="s" s="7">
+      <c r="C45" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D45" t="s" s="7">
+      <c r="D45" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="E45" t="s" s="7">
+      <c r="E45" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-    </row>
-    <row r="46" ht="44.35" customHeight="1">
-      <c r="A46" s="6"/>
-      <c r="B46" t="s" s="7">
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="3"/>
+      <c r="B46" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C46" t="s" s="7">
+      <c r="C46" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D46" t="s" s="7">
+      <c r="D46" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="E46" t="s" s="7">
+      <c r="E46" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-    </row>
-    <row r="47" ht="20.35" customHeight="1">
-      <c r="A47" s="6"/>
-      <c r="B47" t="s" s="7">
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+    </row>
+    <row r="47" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="3"/>
+      <c r="B47" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-    </row>
-    <row r="48" ht="67.1" customHeight="1">
-      <c r="A48" s="6"/>
-      <c r="B48" t="s" s="7">
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+    </row>
+    <row r="48" spans="1:8" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="3"/>
+      <c r="B48" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C48" t="s" s="7">
+      <c r="C48" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D48" t="s" s="7">
+      <c r="D48" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="E48" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E48" t="s" s="7">
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" spans="1:8" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="3"/>
+      <c r="B49" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-    </row>
-    <row r="49" ht="65" customHeight="1">
-      <c r="A49" s="6"/>
-      <c r="B49" t="s" s="7">
+      <c r="C49" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C49" t="s" s="7">
+      <c r="E49" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" spans="1:8" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="3"/>
+      <c r="B50" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+    </row>
+    <row r="51" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="3"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+    </row>
+    <row r="52" spans="1:8" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="3"/>
+      <c r="B52" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+    </row>
+    <row r="53" spans="1:8" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="3"/>
+      <c r="B53" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" spans="1:8" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="3"/>
+      <c r="B54" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+    </row>
+    <row r="55" spans="1:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="3"/>
+      <c r="B55" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+    </row>
+    <row r="56" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="3"/>
+      <c r="B56" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+    </row>
+    <row r="57" spans="1:8" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="3"/>
+      <c r="B57" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+    </row>
+    <row r="58" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="3"/>
+      <c r="B58" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+    </row>
+    <row r="59" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="3"/>
+      <c r="B59" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+    </row>
+    <row r="60" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="3"/>
+      <c r="B60" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+    </row>
+    <row r="61" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="3"/>
+      <c r="B61" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D49" t="s" s="7">
-        <v>142</v>
-      </c>
-      <c r="E49" t="s" s="7">
-        <v>143</v>
-      </c>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-    </row>
-    <row r="50" ht="53" customHeight="1">
-      <c r="A50" s="6"/>
-      <c r="B50" t="s" s="7">
-        <v>144</v>
-      </c>
-      <c r="C50" t="s" s="7">
+      <c r="D61" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+    </row>
+    <row r="62" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="3"/>
+      <c r="B62" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+    </row>
+    <row r="63" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="3"/>
+      <c r="B63" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+    </row>
+    <row r="64" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="3"/>
+      <c r="B64" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+    </row>
+    <row r="65" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="3"/>
+      <c r="B65" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+    </row>
+    <row r="66" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="3"/>
+      <c r="B66" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+    </row>
+    <row r="67" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="3"/>
+      <c r="B67" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C67" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D50" t="s" s="7">
-        <v>145</v>
-      </c>
-      <c r="E50" t="s" s="7">
-        <v>146</v>
-      </c>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-    </row>
-    <row r="51" ht="17" customHeight="1">
-      <c r="A51" s="6"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-    </row>
-    <row r="52" ht="53" customHeight="1">
-      <c r="A52" s="6"/>
-      <c r="B52" t="s" s="7">
-        <v>147</v>
-      </c>
-      <c r="C52" t="s" s="7">
-        <v>106</v>
-      </c>
-      <c r="D52" t="s" s="7">
-        <v>148</v>
-      </c>
-      <c r="E52" t="s" s="7">
-        <v>149</v>
-      </c>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8"/>
-      <c r="H52" s="8"/>
-    </row>
-    <row r="53" ht="53" customHeight="1">
-      <c r="A53" s="6"/>
-      <c r="B53" t="s" s="7">
-        <v>150</v>
-      </c>
-      <c r="C53" t="s" s="7">
-        <v>40</v>
-      </c>
-      <c r="D53" t="s" s="7">
-        <v>151</v>
-      </c>
-      <c r="E53" t="s" s="7">
-        <v>152</v>
-      </c>
-      <c r="F53" s="8"/>
-      <c r="G53" s="8"/>
-      <c r="H53" s="8"/>
-    </row>
-    <row r="54" ht="53" customHeight="1">
-      <c r="A54" s="6"/>
-      <c r="B54" t="s" s="7">
-        <v>153</v>
-      </c>
-      <c r="C54" t="s" s="7">
-        <v>40</v>
-      </c>
-      <c r="D54" t="s" s="7">
-        <v>154</v>
-      </c>
-      <c r="E54" t="s" s="7">
-        <v>155</v>
-      </c>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8"/>
-      <c r="H54" s="8"/>
-    </row>
-    <row r="55" ht="42.65" customHeight="1">
-      <c r="A55" s="6"/>
-      <c r="B55" t="s" s="7">
-        <v>156</v>
-      </c>
-      <c r="C55" t="s" s="7">
-        <v>30</v>
-      </c>
-      <c r="D55" t="s" s="7">
-        <v>157</v>
-      </c>
-      <c r="E55" t="s" s="7">
-        <v>158</v>
-      </c>
-      <c r="F55" s="8"/>
-      <c r="G55" s="8"/>
-      <c r="H55" s="8"/>
-    </row>
-    <row r="56" ht="41" customHeight="1">
-      <c r="A56" s="6"/>
-      <c r="B56" t="s" s="7">
-        <v>159</v>
-      </c>
-      <c r="C56" t="s" s="7">
-        <v>30</v>
-      </c>
-      <c r="D56" t="s" s="7">
-        <v>160</v>
-      </c>
-      <c r="E56" t="s" s="7">
-        <v>155</v>
-      </c>
-      <c r="F56" s="8"/>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
-    </row>
-    <row r="57" ht="53" customHeight="1">
-      <c r="A57" s="6"/>
-      <c r="B57" t="s" s="7">
-        <v>161</v>
-      </c>
-      <c r="C57" t="s" s="7">
-        <v>30</v>
-      </c>
-      <c r="D57" t="s" s="7">
-        <v>162</v>
-      </c>
-      <c r="E57" t="s" s="7">
-        <v>163</v>
-      </c>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8"/>
-      <c r="H57" s="8"/>
-    </row>
-    <row r="58" ht="17" customHeight="1">
-      <c r="A58" s="6"/>
-      <c r="B58" t="s" s="7">
-        <v>164</v>
-      </c>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8"/>
-      <c r="H58" s="8"/>
-    </row>
-    <row r="59" ht="41" customHeight="1">
-      <c r="A59" s="6"/>
-      <c r="B59" t="s" s="7">
-        <v>165</v>
-      </c>
-      <c r="C59" t="s" s="7">
-        <v>166</v>
-      </c>
-      <c r="D59" t="s" s="7">
-        <v>167</v>
-      </c>
-      <c r="E59" t="s" s="7">
-        <v>164</v>
-      </c>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8"/>
-      <c r="H59" s="8"/>
-    </row>
-    <row r="60" ht="17" customHeight="1">
-      <c r="A60" s="6"/>
-      <c r="B60" t="s" s="7">
-        <v>168</v>
-      </c>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="8"/>
-      <c r="G60" s="8"/>
-      <c r="H60" s="8"/>
-    </row>
-    <row r="61" ht="41" customHeight="1">
-      <c r="A61" s="6"/>
-      <c r="B61" t="s" s="7">
-        <v>169</v>
-      </c>
-      <c r="C61" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="D61" t="s" s="7">
-        <v>170</v>
-      </c>
-      <c r="E61" t="s" s="7">
-        <v>168</v>
-      </c>
-      <c r="F61" s="8"/>
-      <c r="G61" s="8"/>
-      <c r="H61" s="8"/>
-    </row>
-    <row r="62" ht="17" customHeight="1">
-      <c r="A62" s="6"/>
-      <c r="B62" t="s" s="7">
-        <v>171</v>
-      </c>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="8"/>
-      <c r="H62" s="8"/>
-    </row>
-    <row r="63" ht="41" customHeight="1">
-      <c r="A63" s="6"/>
-      <c r="B63" t="s" s="7">
-        <v>172</v>
-      </c>
-      <c r="C63" t="s" s="7">
-        <v>166</v>
-      </c>
-      <c r="D63" t="s" s="7">
-        <v>173</v>
-      </c>
-      <c r="E63" t="s" s="7">
-        <v>171</v>
-      </c>
-      <c r="F63" s="8"/>
-      <c r="G63" s="8"/>
-      <c r="H63" s="8"/>
-    </row>
-    <row r="64" ht="17" customHeight="1">
-      <c r="A64" s="6"/>
-      <c r="B64" t="s" s="7">
-        <v>174</v>
-      </c>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="11"/>
-      <c r="F64" s="8"/>
-      <c r="G64" s="8"/>
-      <c r="H64" s="8"/>
-    </row>
-    <row r="65" ht="41" customHeight="1">
-      <c r="A65" s="6"/>
-      <c r="B65" t="s" s="7">
-        <v>175</v>
-      </c>
-      <c r="C65" t="s" s="7">
+      <c r="D67" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+    </row>
+    <row r="68" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="3"/>
+      <c r="B68" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D65" t="s" s="7">
-        <v>176</v>
-      </c>
-      <c r="E65" t="s" s="7">
-        <v>174</v>
-      </c>
-      <c r="F65" s="8"/>
-      <c r="G65" s="8"/>
-      <c r="H65" s="8"/>
-    </row>
-    <row r="66" ht="17" customHeight="1">
-      <c r="A66" s="6"/>
-      <c r="B66" t="s" s="7">
-        <v>177</v>
-      </c>
-      <c r="C66" s="9"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="8"/>
-      <c r="G66" s="8"/>
-      <c r="H66" s="8"/>
-    </row>
-    <row r="67" ht="41" customHeight="1">
-      <c r="A67" s="6"/>
-      <c r="B67" t="s" s="7">
-        <v>178</v>
-      </c>
-      <c r="C67" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="D67" t="s" s="7">
+      <c r="D68" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="E68" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="E67" t="s" s="7">
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+    </row>
+    <row r="69" spans="1:8" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="3"/>
+      <c r="B69" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="F67" s="8"/>
-      <c r="G67" s="8"/>
-      <c r="H67" s="8"/>
-    </row>
-    <row r="68" ht="41" customHeight="1">
-      <c r="A68" s="6"/>
-      <c r="B68" t="s" s="12">
+      <c r="C69" s="11"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+    </row>
+    <row r="70" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="3"/>
+      <c r="B70" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="C68" t="s" s="12">
-        <v>110</v>
-      </c>
-      <c r="D68" t="s" s="7">
+      <c r="C70" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D70" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="E68" t="s" s="12">
+      <c r="E70" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="F68" s="8"/>
-      <c r="G68" s="8"/>
-      <c r="H68" s="8"/>
-    </row>
-    <row r="69" ht="29" customHeight="1">
-      <c r="A69" s="6"/>
-      <c r="B69" t="s" s="13">
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+    </row>
+    <row r="71" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="3"/>
+      <c r="B71" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C69" t="s" s="14">
+      <c r="C71" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D71" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="D69" s="15"/>
-      <c r="E69" s="16"/>
-      <c r="F69" s="8"/>
-      <c r="G69" s="8"/>
-      <c r="H69" s="8"/>
-    </row>
-    <row r="70" ht="41" customHeight="1">
-      <c r="A70" s="6"/>
-      <c r="B70" t="s" s="17">
+      <c r="E71" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="C70" t="s" s="17">
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+    </row>
+    <row r="72" spans="1:8" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="3"/>
+      <c r="B72" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="C72" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D70" t="s" s="17">
-        <v>187</v>
-      </c>
-      <c r="E70" t="s" s="17">
+      <c r="D72" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="F70" s="8"/>
-      <c r="G70" s="8"/>
-      <c r="H70" s="8"/>
-    </row>
-    <row r="71" ht="53" customHeight="1">
-      <c r="A71" s="6"/>
-      <c r="B71" t="s" s="17">
+      <c r="E72" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="C71" t="s" s="17">
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+    </row>
+    <row r="73" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="3"/>
+      <c r="B73" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C73" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D71" t="s" s="17">
-        <v>190</v>
-      </c>
-      <c r="E71" t="s" s="17">
+      <c r="D73" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="E73" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="F71" s="8"/>
-      <c r="G71" s="8"/>
-      <c r="H71" s="8"/>
-    </row>
-    <row r="72" ht="65" customHeight="1">
-      <c r="A72" s="6"/>
-      <c r="B72" t="s" s="17">
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5"/>
+    </row>
+    <row r="74" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="3"/>
+      <c r="B74" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="C72" t="s" s="17">
+      <c r="C74" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D72" t="s" s="17">
+      <c r="D74" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="E72" t="s" s="17">
+      <c r="E74" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="F72" s="8"/>
-      <c r="G72" s="8"/>
-      <c r="H72" s="8"/>
-    </row>
-    <row r="73" ht="53" customHeight="1">
-      <c r="A73" s="6"/>
-      <c r="B73" t="s" s="17">
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+    </row>
+    <row r="75" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="3"/>
+      <c r="B75" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="C73" t="s" s="17">
+      <c r="C75" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E75" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+    </row>
+    <row r="76" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="3"/>
+      <c r="B76" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="C76" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D73" t="s" s="17">
-        <v>196</v>
-      </c>
-      <c r="E73" t="s" s="17">
-        <v>197</v>
-      </c>
-      <c r="F73" s="8"/>
-      <c r="G73" s="8"/>
-      <c r="H73" s="8"/>
-    </row>
-    <row r="74" ht="41" customHeight="1">
-      <c r="A74" s="6"/>
-      <c r="B74" t="s" s="17">
-        <v>198</v>
-      </c>
-      <c r="C74" t="s" s="17">
+      <c r="D76" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="E76" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+    </row>
+    <row r="77" spans="1:8" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="3"/>
+      <c r="B77" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="C77" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D74" t="s" s="17">
-        <v>199</v>
-      </c>
-      <c r="E74" t="s" s="17">
-        <v>200</v>
-      </c>
-      <c r="F74" s="8"/>
-      <c r="G74" s="8"/>
-      <c r="H74" s="8"/>
-    </row>
-    <row r="75" ht="41" customHeight="1">
-      <c r="A75" s="6"/>
-      <c r="B75" t="s" s="17">
-        <v>201</v>
-      </c>
-      <c r="C75" t="s" s="17">
-        <v>202</v>
-      </c>
-      <c r="D75" t="s" s="17">
+      <c r="D77" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="E75" t="s" s="17">
+      <c r="E77" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="F75" s="8"/>
-      <c r="G75" s="8"/>
-      <c r="H75" s="8"/>
-    </row>
-    <row r="76" ht="41" customHeight="1">
-      <c r="A76" s="6"/>
-      <c r="B76" t="s" s="17">
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="5"/>
+    </row>
+    <row r="78" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="3"/>
+      <c r="B78" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="C76" t="s" s="17">
+      <c r="C78" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D76" t="s" s="17">
+      <c r="D78" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="E76" t="s" s="17">
+      <c r="E78" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="F76" s="8"/>
-      <c r="G76" s="8"/>
-      <c r="H76" s="8"/>
-    </row>
-    <row r="77" ht="29" customHeight="1">
-      <c r="A77" s="6"/>
-      <c r="B77" t="s" s="17">
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
+      <c r="H78" s="5"/>
+    </row>
+    <row r="79" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="3"/>
+      <c r="B79" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="C77" t="s" s="17">
+      <c r="C79" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D77" t="s" s="17">
+      <c r="D79" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="E77" t="s" s="17">
+      <c r="E79" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="F77" s="8"/>
-      <c r="G77" s="8"/>
-      <c r="H77" s="8"/>
-    </row>
-    <row r="78" ht="41" customHeight="1">
-      <c r="A78" s="6"/>
-      <c r="B78" t="s" s="17">
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5"/>
+    </row>
+    <row r="80" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="3"/>
+      <c r="B80" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="C78" t="s" s="17">
+      <c r="C80" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D78" t="s" s="17">
+      <c r="D80" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="E78" t="s" s="17">
+      <c r="E80" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="F78" s="8"/>
-      <c r="G78" s="8"/>
-      <c r="H78" s="8"/>
-    </row>
-    <row r="79" ht="41" customHeight="1">
-      <c r="A79" s="6"/>
-      <c r="B79" t="s" s="17">
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5"/>
+    </row>
+    <row r="81" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="3"/>
+      <c r="B81" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="C79" t="s" s="17">
+      <c r="C81" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D81" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="E81" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="F81" s="15"/>
+      <c r="G81" s="5"/>
+      <c r="H81" s="5"/>
+    </row>
+    <row r="82" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="3"/>
+      <c r="B82" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="E82" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="F82" s="15"/>
+      <c r="G82" s="5"/>
+      <c r="H82" s="5"/>
+    </row>
+    <row r="83" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="3"/>
+      <c r="B83" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="E83" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="F83" s="15"/>
+      <c r="G83" s="5"/>
+      <c r="H83" s="5"/>
+    </row>
+    <row r="84" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="3"/>
+      <c r="B84" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="C84" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="E84" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="F84" s="15"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
+    </row>
+    <row r="85" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="3"/>
+      <c r="B85" s="14"/>
+      <c r="C85" s="14"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="15"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="5"/>
+    </row>
+    <row r="86" spans="1:8" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="3"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="14"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="15"/>
+      <c r="G86" s="5"/>
+      <c r="H86" s="5"/>
+    </row>
+    <row r="87" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="3"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="14"/>
+      <c r="D87" s="14"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="15"/>
+      <c r="G87" s="5"/>
+      <c r="H87" s="5"/>
+    </row>
+    <row r="88" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="3"/>
+      <c r="B88" s="14"/>
+      <c r="C88" s="14"/>
+      <c r="D88" s="14"/>
+      <c r="E88" s="14"/>
+      <c r="F88" s="15"/>
+      <c r="G88" s="5"/>
+      <c r="H88" s="5"/>
+    </row>
+    <row r="89" spans="1:8" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="3"/>
+      <c r="B89" s="14"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="15"/>
+      <c r="G89" s="5"/>
+      <c r="H89" s="5"/>
+    </row>
+    <row r="90" spans="1:8" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="3"/>
+      <c r="B90" s="14"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="15"/>
+      <c r="G90" s="5"/>
+      <c r="H90" s="5"/>
+    </row>
+    <row r="91" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="3"/>
+      <c r="B91" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="C91" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D91" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="E91" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="F91" s="15"/>
+      <c r="G91" s="5"/>
+      <c r="H91" s="5"/>
+    </row>
+    <row r="92" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="3"/>
+      <c r="B92" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="C92" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D92" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="E92" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="F92" s="15"/>
+      <c r="G92" s="5"/>
+      <c r="H92" s="5"/>
+    </row>
+    <row r="93" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="3"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="15"/>
+      <c r="G93" s="5"/>
+      <c r="H93" s="5"/>
+    </row>
+    <row r="94" spans="1:8" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="3"/>
+      <c r="B94" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C94" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D79" t="s" s="17">
-        <v>215</v>
-      </c>
-      <c r="E79" t="s" s="17">
-        <v>216</v>
-      </c>
-      <c r="F79" s="8"/>
-      <c r="G79" s="8"/>
-      <c r="H79" s="8"/>
-    </row>
-    <row r="80" ht="41" customHeight="1">
-      <c r="A80" s="6"/>
-      <c r="B80" t="s" s="17">
-        <v>217</v>
-      </c>
-      <c r="C80" t="s" s="17">
+      <c r="D94" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="F94" s="15"/>
+      <c r="G94" s="5"/>
+      <c r="H94" s="5"/>
+    </row>
+    <row r="95" spans="1:8" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="3"/>
+      <c r="B95" s="9"/>
+      <c r="C95" s="8"/>
+      <c r="D95" s="8"/>
+      <c r="E95" s="8"/>
+      <c r="F95" s="15"/>
+      <c r="G95" s="5"/>
+      <c r="H95" s="5"/>
+    </row>
+    <row r="96" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="3"/>
+      <c r="B96" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="C96" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D80" t="s" s="17">
-        <v>218</v>
-      </c>
-      <c r="E80" t="s" s="17">
-        <v>219</v>
-      </c>
-      <c r="F80" s="8"/>
-      <c r="G80" s="8"/>
-      <c r="H80" s="8"/>
-    </row>
-    <row r="81" ht="41" customHeight="1">
-      <c r="A81" s="6"/>
-      <c r="B81" t="s" s="17">
-        <v>220</v>
-      </c>
-      <c r="C81" t="s" s="17">
-        <v>113</v>
-      </c>
-      <c r="D81" t="s" s="17">
-        <v>221</v>
-      </c>
-      <c r="E81" t="s" s="17">
-        <v>222</v>
-      </c>
-      <c r="F81" s="18"/>
-      <c r="G81" s="8"/>
-      <c r="H81" s="8"/>
-    </row>
-    <row r="82" ht="41" customHeight="1">
-      <c r="A82" s="6"/>
-      <c r="B82" t="s" s="17">
-        <v>223</v>
-      </c>
-      <c r="C82" t="s" s="17">
-        <v>113</v>
-      </c>
-      <c r="D82" t="s" s="17">
-        <v>224</v>
-      </c>
-      <c r="E82" t="s" s="17">
-        <v>225</v>
-      </c>
-      <c r="F82" s="18"/>
-      <c r="G82" s="8"/>
-      <c r="H82" s="8"/>
-    </row>
-    <row r="83" ht="53" customHeight="1">
-      <c r="A83" s="6"/>
-      <c r="B83" t="s" s="17">
-        <v>226</v>
-      </c>
-      <c r="C83" t="s" s="17">
-        <v>113</v>
-      </c>
-      <c r="D83" t="s" s="17">
-        <v>227</v>
-      </c>
-      <c r="E83" t="s" s="17">
-        <v>228</v>
-      </c>
-      <c r="F83" s="18"/>
-      <c r="G83" s="8"/>
-      <c r="H83" s="8"/>
-    </row>
-    <row r="84" ht="41" customHeight="1">
-      <c r="A84" s="6"/>
-      <c r="B84" t="s" s="17">
-        <v>229</v>
-      </c>
-      <c r="C84" t="s" s="17">
-        <v>113</v>
-      </c>
-      <c r="D84" t="s" s="17">
-        <v>230</v>
-      </c>
-      <c r="E84" t="s" s="17">
-        <v>231</v>
-      </c>
-      <c r="F84" s="18"/>
-      <c r="G84" s="8"/>
-      <c r="H84" s="8"/>
-    </row>
-    <row r="85" ht="41" customHeight="1">
-      <c r="A85" s="6"/>
-      <c r="B85" t="s" s="17">
-        <v>232</v>
-      </c>
-      <c r="C85" t="s" s="17">
-        <v>113</v>
-      </c>
-      <c r="D85" t="s" s="17">
-        <v>233</v>
-      </c>
-      <c r="E85" t="s" s="17">
-        <v>234</v>
-      </c>
-      <c r="F85" s="18"/>
-      <c r="G85" s="8"/>
-      <c r="H85" s="8"/>
-    </row>
-    <row r="86" ht="29" customHeight="1">
-      <c r="A86" s="6"/>
-      <c r="B86" t="s" s="17">
-        <v>235</v>
-      </c>
-      <c r="C86" t="s" s="17">
-        <v>113</v>
-      </c>
-      <c r="D86" t="s" s="17">
-        <v>209</v>
-      </c>
-      <c r="E86" t="s" s="17">
+      <c r="D96" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="E96" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="F86" s="18"/>
-      <c r="G86" s="8"/>
-      <c r="H86" s="8"/>
-    </row>
-    <row r="87" ht="41" customHeight="1">
-      <c r="A87" s="6"/>
-      <c r="B87" t="s" s="17">
+      <c r="F96" s="15"/>
+      <c r="G96" s="5"/>
+      <c r="H96" s="5"/>
+    </row>
+    <row r="97" spans="1:8" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="3"/>
+      <c r="B97" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="C87" t="s" s="17">
-        <v>113</v>
-      </c>
-      <c r="D87" t="s" s="17">
-        <v>212</v>
-      </c>
-      <c r="E87" t="s" s="17">
+      <c r="C97" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D97" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="F87" s="18"/>
-      <c r="G87" s="8"/>
-      <c r="H87" s="8"/>
-    </row>
-    <row r="88" ht="41" customHeight="1">
-      <c r="A88" s="6"/>
-      <c r="B88" t="s" s="17">
+      <c r="E97" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="C88" t="s" s="17">
-        <v>113</v>
-      </c>
-      <c r="D88" t="s" s="17">
-        <v>215</v>
-      </c>
-      <c r="E88" t="s" s="17">
+      <c r="F97" s="15"/>
+      <c r="G97" s="5"/>
+      <c r="H97" s="5"/>
+    </row>
+    <row r="98" spans="1:8" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="3"/>
+      <c r="B98" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="F88" s="18"/>
-      <c r="G88" s="8"/>
-      <c r="H88" s="8"/>
-    </row>
-    <row r="89" ht="29" customHeight="1">
-      <c r="A89" s="6"/>
-      <c r="B89" t="s" s="17">
+      <c r="C98" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D98" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="C89" t="s" s="17">
-        <v>113</v>
-      </c>
-      <c r="D89" t="s" s="17">
+      <c r="E98" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="F98" s="15"/>
+      <c r="G98" s="5"/>
+      <c r="H98" s="5"/>
+    </row>
+    <row r="99" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="3"/>
+      <c r="B99" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="E89" t="s" s="17">
+      <c r="C99" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D99" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="F89" s="18"/>
-      <c r="G89" s="8"/>
-      <c r="H89" s="8"/>
-    </row>
-    <row r="90" ht="29" customHeight="1">
-      <c r="A90" s="6"/>
-      <c r="B90" t="s" s="17">
+      <c r="E99" s="14" t="s">
         <v>244</v>
       </c>
-      <c r="C90" t="s" s="17">
-        <v>113</v>
-      </c>
-      <c r="D90" t="s" s="17">
+      <c r="F99" s="15"/>
+      <c r="G99" s="5"/>
+      <c r="H99" s="5"/>
+    </row>
+    <row r="100" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="3"/>
+      <c r="B100" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="E90" t="s" s="17">
+      <c r="C100" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D100" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="F90" s="18"/>
-      <c r="G90" s="8"/>
-      <c r="H90" s="8"/>
-    </row>
-    <row r="91" ht="41" customHeight="1">
-      <c r="A91" s="6"/>
-      <c r="B91" t="s" s="17">
+      <c r="E100" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="C91" t="s" s="17">
-        <v>113</v>
-      </c>
-      <c r="D91" t="s" s="17">
+      <c r="F100" s="15"/>
+      <c r="G100" s="5"/>
+      <c r="H100" s="5"/>
+    </row>
+    <row r="101" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="3"/>
+      <c r="B101" s="14" t="s">
         <v>248</v>
       </c>
-      <c r="E91" t="s" s="17">
+      <c r="C101" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D101" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="F91" s="18"/>
-      <c r="G91" s="8"/>
-      <c r="H91" s="8"/>
-    </row>
-    <row r="92" ht="53" customHeight="1">
-      <c r="A92" s="6"/>
-      <c r="B92" t="s" s="17">
+      <c r="E101" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="C92" t="s" s="17">
-        <v>113</v>
-      </c>
-      <c r="D92" t="s" s="17">
+      <c r="F101" s="15"/>
+      <c r="G101" s="5"/>
+      <c r="H101" s="5"/>
+    </row>
+    <row r="102" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="3"/>
+      <c r="B102" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="E92" t="s" s="17">
+      <c r="C102" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D102" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="F92" s="18"/>
-      <c r="G92" s="8"/>
-      <c r="H92" s="8"/>
-    </row>
-    <row r="93" ht="17" customHeight="1">
-      <c r="A93" s="6"/>
-      <c r="B93" t="s" s="7">
+      <c r="E102" s="14" t="s">
         <v>253</v>
       </c>
-      <c r="C93" s="9"/>
-      <c r="D93" s="9"/>
-      <c r="E93" s="9"/>
-      <c r="F93" s="18"/>
-      <c r="G93" s="8"/>
-      <c r="H93" s="8"/>
-    </row>
-    <row r="94" ht="53" customHeight="1">
-      <c r="A94" s="6"/>
-      <c r="B94" t="s" s="7">
+      <c r="F102" s="15"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="5"/>
+    </row>
+    <row r="103" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="3"/>
+      <c r="B103" s="14" t="s">
         <v>254</v>
       </c>
-      <c r="C94" t="s" s="7">
+      <c r="C103" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D94" t="s" s="7">
+      <c r="D103" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="E94" t="s" s="7">
-        <v>253</v>
-      </c>
-      <c r="F94" s="18"/>
-      <c r="G94" s="8"/>
-      <c r="H94" s="8"/>
-    </row>
-    <row r="95" ht="29" customHeight="1">
-      <c r="A95" s="6"/>
-      <c r="B95" t="s" s="12">
+      <c r="E103" s="14" t="s">
         <v>256</v>
       </c>
-      <c r="C95" s="11"/>
-      <c r="D95" s="11"/>
-      <c r="E95" s="11"/>
-      <c r="F95" s="18"/>
-      <c r="G95" s="8"/>
-      <c r="H95" s="8"/>
-    </row>
-    <row r="96" ht="41" customHeight="1">
-      <c r="A96" s="6"/>
-      <c r="B96" t="s" s="17">
+      <c r="F103" s="15"/>
+      <c r="G103" s="5"/>
+      <c r="H103" s="5"/>
+    </row>
+    <row r="104" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="3"/>
+      <c r="B104" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="C96" t="s" s="17">
+      <c r="C104" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D96" t="s" s="17">
+      <c r="D104" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="E96" t="s" s="17">
+      <c r="E104" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="F96" s="18"/>
-      <c r="G96" s="8"/>
-      <c r="H96" s="8"/>
-    </row>
-    <row r="97" ht="53" customHeight="1">
-      <c r="A97" s="6"/>
-      <c r="B97" t="s" s="17">
+      <c r="F104" s="15"/>
+      <c r="G104" s="5"/>
+      <c r="H104" s="5"/>
+    </row>
+    <row r="105" spans="1:8" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="3"/>
+      <c r="B105" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C97" t="s" s="17">
+      <c r="C105" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D97" t="s" s="17">
+      <c r="D105" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="E97" t="s" s="17">
+      <c r="E105" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="F97" s="18"/>
-      <c r="G97" s="8"/>
-      <c r="H97" s="8"/>
-    </row>
-    <row r="98" ht="53" customHeight="1">
-      <c r="A98" s="6"/>
-      <c r="B98" t="s" s="17">
+      <c r="F105" s="15"/>
+      <c r="G105" s="5"/>
+      <c r="H105" s="5"/>
+    </row>
+    <row r="106" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="3"/>
+      <c r="B106" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="C98" t="s" s="17">
+      <c r="C106" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D98" t="s" s="17">
+      <c r="D106" s="14" t="s">
         <v>264</v>
       </c>
-      <c r="E98" t="s" s="17">
-        <v>262</v>
-      </c>
-      <c r="F98" s="18"/>
-      <c r="G98" s="8"/>
-      <c r="H98" s="8"/>
-    </row>
-    <row r="99" ht="41" customHeight="1">
-      <c r="A99" s="6"/>
-      <c r="B99" t="s" s="17">
+      <c r="E106" s="14" t="s">
         <v>265</v>
       </c>
-      <c r="C99" t="s" s="17">
+      <c r="F106" s="15"/>
+      <c r="G106" s="5"/>
+      <c r="H106" s="5"/>
+    </row>
+    <row r="107" spans="1:8" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="3"/>
+      <c r="B107" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="C107" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D99" t="s" s="17">
-        <v>266</v>
-      </c>
-      <c r="E99" t="s" s="17">
+      <c r="D107" s="14" t="s">
         <v>267</v>
       </c>
-      <c r="F99" s="18"/>
-      <c r="G99" s="8"/>
-      <c r="H99" s="8"/>
-    </row>
-    <row r="100" ht="41" customHeight="1">
-      <c r="A100" s="6"/>
-      <c r="B100" t="s" s="17">
+      <c r="E107" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="C100" t="s" s="17">
+      <c r="F107" s="15"/>
+      <c r="G107" s="5"/>
+      <c r="H107" s="5"/>
+    </row>
+    <row r="108" spans="1:8" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="3"/>
+      <c r="B108" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C108" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D100" t="s" s="17">
-        <v>269</v>
-      </c>
-      <c r="E100" t="s" s="17">
+      <c r="D108" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F100" s="18"/>
-      <c r="G100" s="8"/>
-      <c r="H100" s="8"/>
-    </row>
-    <row r="101" ht="41" customHeight="1">
-      <c r="A101" s="6"/>
-      <c r="B101" t="s" s="17">
+      <c r="E108" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="C101" t="s" s="17">
+      <c r="F108" s="15"/>
+      <c r="G108" s="5"/>
+      <c r="H108" s="5"/>
+    </row>
+    <row r="109" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="3"/>
+      <c r="B109" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="C109" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D101" t="s" s="17">
-        <v>272</v>
-      </c>
-      <c r="E101" t="s" s="17">
+      <c r="D109" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="F101" s="18"/>
-      <c r="G101" s="8"/>
-      <c r="H101" s="8"/>
-    </row>
-    <row r="102" ht="41" customHeight="1">
-      <c r="A102" s="6"/>
-      <c r="B102" t="s" s="17">
+      <c r="E109" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="C102" t="s" s="17">
-        <v>26</v>
-      </c>
-      <c r="D102" t="s" s="17">
-        <v>275</v>
-      </c>
-      <c r="E102" t="s" s="17">
-        <v>276</v>
-      </c>
-      <c r="F102" s="18"/>
-      <c r="G102" s="8"/>
-      <c r="H102" s="8"/>
-    </row>
-    <row r="103" ht="53" customHeight="1">
-      <c r="A103" s="6"/>
-      <c r="B103" t="s" s="17">
-        <v>277</v>
-      </c>
-      <c r="C103" t="s" s="17">
-        <v>26</v>
-      </c>
-      <c r="D103" t="s" s="17">
-        <v>278</v>
-      </c>
-      <c r="E103" t="s" s="17">
-        <v>279</v>
-      </c>
-      <c r="F103" s="18"/>
-      <c r="G103" s="8"/>
-      <c r="H103" s="8"/>
-    </row>
-    <row r="104" ht="41" customHeight="1">
-      <c r="A104" s="6"/>
-      <c r="B104" t="s" s="17">
-        <v>280</v>
-      </c>
-      <c r="C104" t="s" s="17">
-        <v>26</v>
-      </c>
-      <c r="D104" t="s" s="17">
-        <v>281</v>
-      </c>
-      <c r="E104" t="s" s="17">
-        <v>282</v>
-      </c>
-      <c r="F104" s="18"/>
-      <c r="G104" s="8"/>
-      <c r="H104" s="8"/>
-    </row>
-    <row r="105" ht="53" customHeight="1">
-      <c r="A105" s="6"/>
-      <c r="B105" t="s" s="17">
-        <v>283</v>
-      </c>
-      <c r="C105" t="s" s="17">
-        <v>26</v>
-      </c>
-      <c r="D105" t="s" s="17">
-        <v>284</v>
-      </c>
-      <c r="E105" t="s" s="17">
-        <v>285</v>
-      </c>
-      <c r="F105" s="18"/>
-      <c r="G105" s="8"/>
-      <c r="H105" s="8"/>
-    </row>
-    <row r="106" ht="41" customHeight="1">
-      <c r="A106" s="6"/>
-      <c r="B106" t="s" s="17">
-        <v>286</v>
-      </c>
-      <c r="C106" t="s" s="17">
-        <v>26</v>
-      </c>
-      <c r="D106" t="s" s="17">
-        <v>287</v>
-      </c>
-      <c r="E106" t="s" s="17">
-        <v>288</v>
-      </c>
-      <c r="F106" s="18"/>
-      <c r="G106" s="8"/>
-      <c r="H106" s="8"/>
-    </row>
-    <row r="107" ht="53" customHeight="1">
-      <c r="A107" s="6"/>
-      <c r="B107" t="s" s="17">
-        <v>289</v>
-      </c>
-      <c r="C107" t="s" s="17">
-        <v>26</v>
-      </c>
-      <c r="D107" t="s" s="17">
-        <v>290</v>
-      </c>
-      <c r="E107" t="s" s="17">
-        <v>291</v>
-      </c>
-      <c r="F107" s="18"/>
-      <c r="G107" s="8"/>
-      <c r="H107" s="8"/>
-    </row>
-    <row r="108" ht="65" customHeight="1">
-      <c r="A108" s="6"/>
-      <c r="B108" t="s" s="17">
-        <v>292</v>
-      </c>
-      <c r="C108" t="s" s="17">
-        <v>26</v>
-      </c>
-      <c r="D108" t="s" s="17">
-        <v>293</v>
-      </c>
-      <c r="E108" t="s" s="17">
-        <v>294</v>
-      </c>
-      <c r="F108" s="18"/>
-      <c r="G108" s="8"/>
-      <c r="H108" s="8"/>
-    </row>
-    <row r="109" ht="41" customHeight="1">
-      <c r="A109" s="6"/>
-      <c r="B109" t="s" s="17">
-        <v>295</v>
-      </c>
-      <c r="C109" t="s" s="17">
-        <v>26</v>
-      </c>
-      <c r="D109" t="s" s="17">
-        <v>296</v>
-      </c>
-      <c r="E109" t="s" s="17">
-        <v>297</v>
-      </c>
-      <c r="F109" s="18"/>
-      <c r="G109" s="8"/>
-      <c r="H109" s="8"/>
+      <c r="F109" s="15"/>
+      <c r="G109" s="5"/>
+      <c r="H109" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>

</xml_diff>